<commit_message>
Texas Candidates' Twitter Follower Outputs
Output of analysis for Texas. Future analyses will utilize a SQL database, rather than writing to .csv files.
</commit_message>
<xml_diff>
--- a/election_calendar/federal_election_info.xlsx
+++ b/election_calendar/federal_election_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amedeloitte-my.sharepoint.com/personal/kohayward_deloitte_com/Documents/Desktop/federal_election_social_bot_analysis/election_calendar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="8_{A3BCC114-850C-9C4D-B7F8-5A23C477092A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D5D8BB4-9B20-4A91-A438-E9FEC1F6269E}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="8_{A3BCC114-850C-9C4D-B7F8-5A23C477092A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{A27A4739-70EA-49CC-B514-C124EAF36FD7}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="21315" yWindow="2460" windowWidth="32355" windowHeight="17235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21315" yWindow="2460" windowWidth="32355" windowHeight="17235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -642,7 +642,7 @@
   <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,6 +651,7 @@
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" customWidth="1"/>
     <col min="6" max="6" width="41.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="42.140625" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>